<commit_message>
na for sub category data
</commit_message>
<xml_diff>
--- a/data/ece-catalog.xlsx
+++ b/data/ece-catalog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Elisa/Documents/uwece-catalog/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1D5D4F7-252B-1843-AF71-030D40D4C94B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{390B90D2-31A0-2C44-9FFB-0DD992C2E261}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10820" yWindow="460" windowWidth="14780" windowHeight="14180" xr2:uid="{0B1F95D0-FD8F-8249-8FAE-3C2EA3F05EE2}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2872" uniqueCount="1545">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3178" uniqueCount="1546">
   <si>
     <t>Part #</t>
   </si>
@@ -4660,6 +4660,9 @@
   </si>
   <si>
     <t>Blank CDR</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -5077,8 +5080,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B127431A-815B-8C47-B798-29A98F3159CA}">
   <dimension ref="A1:H797"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A92" workbookViewId="0">
-      <selection activeCell="C109" sqref="C109"/>
+    <sheetView tabSelected="1" topLeftCell="A769" workbookViewId="0">
+      <selection activeCell="D788" sqref="D788"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13763,6 +13766,9 @@
       <c r="B492" s="7" t="s">
         <v>943</v>
       </c>
+      <c r="C492" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D492" t="s">
         <v>944</v>
       </c>
@@ -13777,6 +13783,9 @@
       <c r="B493" s="7" t="s">
         <v>943</v>
       </c>
+      <c r="C493" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D493" t="s">
         <v>945</v>
       </c>
@@ -13791,6 +13800,9 @@
       <c r="B494" s="7" t="s">
         <v>943</v>
       </c>
+      <c r="C494" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D494" t="s">
         <v>946</v>
       </c>
@@ -13805,6 +13817,9 @@
       <c r="B495" s="7" t="s">
         <v>943</v>
       </c>
+      <c r="C495" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D495" t="s">
         <v>947</v>
       </c>
@@ -13819,6 +13834,9 @@
       <c r="B496" s="7" t="s">
         <v>943</v>
       </c>
+      <c r="C496" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D496" t="s">
         <v>948</v>
       </c>
@@ -13833,6 +13851,9 @@
       <c r="B497" s="7" t="s">
         <v>943</v>
       </c>
+      <c r="C497" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D497" t="s">
         <v>949</v>
       </c>
@@ -13847,6 +13868,9 @@
       <c r="B498" s="7" t="s">
         <v>943</v>
       </c>
+      <c r="C498" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D498" t="s">
         <v>950</v>
       </c>
@@ -13861,6 +13885,9 @@
       <c r="B499" s="7" t="s">
         <v>943</v>
       </c>
+      <c r="C499" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D499" t="s">
         <v>951</v>
       </c>
@@ -13875,6 +13902,9 @@
       <c r="B500" s="7" t="s">
         <v>943</v>
       </c>
+      <c r="C500" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D500" t="s">
         <v>952</v>
       </c>
@@ -13889,6 +13919,9 @@
       <c r="B501" s="7" t="s">
         <v>943</v>
       </c>
+      <c r="C501" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D501" t="s">
         <v>953</v>
       </c>
@@ -13903,6 +13936,9 @@
       <c r="B502" s="7" t="s">
         <v>943</v>
       </c>
+      <c r="C502" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D502" t="s">
         <v>954</v>
       </c>
@@ -13917,6 +13953,9 @@
       <c r="B503" s="7" t="s">
         <v>943</v>
       </c>
+      <c r="C503" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D503" t="s">
         <v>955</v>
       </c>
@@ -13931,6 +13970,9 @@
       <c r="B504" s="7" t="s">
         <v>943</v>
       </c>
+      <c r="C504" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D504" t="s">
         <v>956</v>
       </c>
@@ -13945,6 +13987,9 @@
       <c r="B505" s="7" t="s">
         <v>943</v>
       </c>
+      <c r="C505" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D505" t="s">
         <v>957</v>
       </c>
@@ -13959,6 +14004,9 @@
       <c r="B506" s="7" t="s">
         <v>943</v>
       </c>
+      <c r="C506" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D506" t="s">
         <v>958</v>
       </c>
@@ -13973,6 +14021,9 @@
       <c r="B507" s="7" t="s">
         <v>943</v>
       </c>
+      <c r="C507" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D507" t="s">
         <v>959</v>
       </c>
@@ -13987,6 +14038,9 @@
       <c r="B508" s="7" t="s">
         <v>943</v>
       </c>
+      <c r="C508" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D508" t="s">
         <v>960</v>
       </c>
@@ -14001,6 +14055,9 @@
       <c r="B509" s="7" t="s">
         <v>943</v>
       </c>
+      <c r="C509" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D509" t="s">
         <v>961</v>
       </c>
@@ -14015,6 +14072,9 @@
       <c r="B510" s="7" t="s">
         <v>943</v>
       </c>
+      <c r="C510" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D510" t="s">
         <v>962</v>
       </c>
@@ -14029,6 +14089,9 @@
       <c r="B511" s="7" t="s">
         <v>943</v>
       </c>
+      <c r="C511" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D511" t="s">
         <v>963</v>
       </c>
@@ -14043,6 +14106,9 @@
       <c r="B512" s="7" t="s">
         <v>943</v>
       </c>
+      <c r="C512" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D512" t="s">
         <v>964</v>
       </c>
@@ -14057,6 +14123,9 @@
       <c r="B513" s="7" t="s">
         <v>943</v>
       </c>
+      <c r="C513" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D513" t="s">
         <v>965</v>
       </c>
@@ -14071,6 +14140,9 @@
       <c r="B514" s="7" t="s">
         <v>943</v>
       </c>
+      <c r="C514" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D514" t="s">
         <v>966</v>
       </c>
@@ -14085,6 +14157,9 @@
       <c r="B515" s="7" t="s">
         <v>943</v>
       </c>
+      <c r="C515" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D515" t="s">
         <v>967</v>
       </c>
@@ -14099,6 +14174,9 @@
       <c r="B516" s="7" t="s">
         <v>943</v>
       </c>
+      <c r="C516" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D516" t="s">
         <v>968</v>
       </c>
@@ -14113,6 +14191,9 @@
       <c r="B517" s="7" t="s">
         <v>943</v>
       </c>
+      <c r="C517" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D517" t="s">
         <v>969</v>
       </c>
@@ -14127,6 +14208,9 @@
       <c r="B518" s="7" t="s">
         <v>943</v>
       </c>
+      <c r="C518" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D518" t="s">
         <v>970</v>
       </c>
@@ -14141,6 +14225,9 @@
       <c r="B519" s="7" t="s">
         <v>943</v>
       </c>
+      <c r="C519" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D519" t="s">
         <v>971</v>
       </c>
@@ -14155,6 +14242,9 @@
       <c r="B520" s="7" t="s">
         <v>943</v>
       </c>
+      <c r="C520" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D520" t="s">
         <v>972</v>
       </c>
@@ -14169,6 +14259,9 @@
       <c r="B521" s="7" t="s">
         <v>943</v>
       </c>
+      <c r="C521" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D521" t="s">
         <v>973</v>
       </c>
@@ -14183,6 +14276,9 @@
       <c r="B522" s="7" t="s">
         <v>943</v>
       </c>
+      <c r="C522" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D522" t="s">
         <v>974</v>
       </c>
@@ -14197,6 +14293,9 @@
       <c r="B523" s="7" t="s">
         <v>943</v>
       </c>
+      <c r="C523" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D523" t="s">
         <v>975</v>
       </c>
@@ -14211,6 +14310,9 @@
       <c r="B524" s="7" t="s">
         <v>943</v>
       </c>
+      <c r="C524" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D524" t="s">
         <v>976</v>
       </c>
@@ -14225,6 +14327,9 @@
       <c r="B525" s="7" t="s">
         <v>943</v>
       </c>
+      <c r="C525" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D525" t="s">
         <v>977</v>
       </c>
@@ -14239,6 +14344,9 @@
       <c r="B526" s="7" t="s">
         <v>943</v>
       </c>
+      <c r="C526" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D526" t="s">
         <v>978</v>
       </c>
@@ -14253,6 +14361,9 @@
       <c r="B527" s="7" t="s">
         <v>943</v>
       </c>
+      <c r="C527" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D527" t="s">
         <v>979</v>
       </c>
@@ -14267,6 +14378,9 @@
       <c r="B528" s="7" t="s">
         <v>943</v>
       </c>
+      <c r="C528" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D528" t="s">
         <v>1013</v>
       </c>
@@ -14281,6 +14395,9 @@
       <c r="B529" s="7" t="s">
         <v>943</v>
       </c>
+      <c r="C529" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D529" t="s">
         <v>1014</v>
       </c>
@@ -14295,6 +14412,9 @@
       <c r="B530" s="7" t="s">
         <v>943</v>
       </c>
+      <c r="C530" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D530" t="s">
         <v>1015</v>
       </c>
@@ -14309,6 +14429,9 @@
       <c r="B531" s="7" t="s">
         <v>943</v>
       </c>
+      <c r="C531" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D531" t="s">
         <v>1016</v>
       </c>
@@ -14323,6 +14446,9 @@
       <c r="B532" s="7" t="s">
         <v>943</v>
       </c>
+      <c r="C532" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D532" t="s">
         <v>1017</v>
       </c>
@@ -14337,6 +14463,9 @@
       <c r="B533" s="7" t="s">
         <v>943</v>
       </c>
+      <c r="C533" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D533" t="s">
         <v>1018</v>
       </c>
@@ -14351,6 +14480,9 @@
       <c r="B534" s="7" t="s">
         <v>943</v>
       </c>
+      <c r="C534" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D534" t="s">
         <v>1019</v>
       </c>
@@ -14365,6 +14497,9 @@
       <c r="B535" s="7" t="s">
         <v>943</v>
       </c>
+      <c r="C535" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D535" t="s">
         <v>1020</v>
       </c>
@@ -14379,6 +14514,9 @@
       <c r="B536" s="7" t="s">
         <v>943</v>
       </c>
+      <c r="C536" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D536" t="s">
         <v>1021</v>
       </c>
@@ -14393,6 +14531,9 @@
       <c r="B537" s="7" t="s">
         <v>943</v>
       </c>
+      <c r="C537" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D537" t="s">
         <v>1022</v>
       </c>
@@ -14407,6 +14548,9 @@
       <c r="B538" s="7" t="s">
         <v>943</v>
       </c>
+      <c r="C538" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D538" t="s">
         <v>1023</v>
       </c>
@@ -14421,6 +14565,9 @@
       <c r="B539" s="7" t="s">
         <v>943</v>
       </c>
+      <c r="C539" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D539" t="s">
         <v>1024</v>
       </c>
@@ -14435,6 +14582,9 @@
       <c r="B540" s="7" t="s">
         <v>943</v>
       </c>
+      <c r="C540" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D540" t="s">
         <v>1025</v>
       </c>
@@ -14449,6 +14599,9 @@
       <c r="B541" s="7" t="s">
         <v>943</v>
       </c>
+      <c r="C541" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D541" t="s">
         <v>1026</v>
       </c>
@@ -14463,6 +14616,9 @@
       <c r="B542" s="7" t="s">
         <v>943</v>
       </c>
+      <c r="C542" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D542" t="s">
         <v>1027</v>
       </c>
@@ -14477,6 +14633,9 @@
       <c r="B543" s="7" t="s">
         <v>943</v>
       </c>
+      <c r="C543" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D543" t="s">
         <v>1028</v>
       </c>
@@ -14491,6 +14650,9 @@
       <c r="B544" s="7" t="s">
         <v>943</v>
       </c>
+      <c r="C544" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D544" t="s">
         <v>1029</v>
       </c>
@@ -14505,6 +14667,9 @@
       <c r="B545" s="7" t="s">
         <v>943</v>
       </c>
+      <c r="C545" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D545" t="s">
         <v>1030</v>
       </c>
@@ -14519,6 +14684,9 @@
       <c r="B546" s="7" t="s">
         <v>943</v>
       </c>
+      <c r="C546" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D546" t="s">
         <v>1031</v>
       </c>
@@ -14533,6 +14701,9 @@
       <c r="B547" s="7" t="s">
         <v>943</v>
       </c>
+      <c r="C547" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D547" t="s">
         <v>1032</v>
       </c>
@@ -14544,6 +14715,9 @@
       <c r="B548" s="7" t="s">
         <v>943</v>
       </c>
+      <c r="C548" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D548" t="s">
         <v>1033</v>
       </c>
@@ -14558,6 +14732,9 @@
       <c r="B549" s="7" t="s">
         <v>943</v>
       </c>
+      <c r="C549" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D549" t="s">
         <v>1034</v>
       </c>
@@ -14572,6 +14749,9 @@
       <c r="B550" s="7" t="s">
         <v>943</v>
       </c>
+      <c r="C550" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D550" t="s">
         <v>1035</v>
       </c>
@@ -14586,6 +14766,9 @@
       <c r="B551" s="7" t="s">
         <v>943</v>
       </c>
+      <c r="C551" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D551" t="s">
         <v>1036</v>
       </c>
@@ -14600,6 +14783,9 @@
       <c r="B552" s="7" t="s">
         <v>943</v>
       </c>
+      <c r="C552" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D552" t="s">
         <v>1037</v>
       </c>
@@ -14614,6 +14800,9 @@
       <c r="B553" s="7" t="s">
         <v>943</v>
       </c>
+      <c r="C553" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D553" t="s">
         <v>1038</v>
       </c>
@@ -14628,6 +14817,9 @@
       <c r="B554" s="7" t="s">
         <v>943</v>
       </c>
+      <c r="C554" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D554" t="s">
         <v>1039</v>
       </c>
@@ -14642,6 +14834,9 @@
       <c r="B555" s="7" t="s">
         <v>943</v>
       </c>
+      <c r="C555" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D555" t="s">
         <v>1040</v>
       </c>
@@ -14656,6 +14851,9 @@
       <c r="B556" s="7" t="s">
         <v>943</v>
       </c>
+      <c r="C556" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D556" t="s">
         <v>1041</v>
       </c>
@@ -14670,6 +14868,9 @@
       <c r="B557" s="7" t="s">
         <v>943</v>
       </c>
+      <c r="C557" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D557" t="s">
         <v>1042</v>
       </c>
@@ -14684,6 +14885,9 @@
       <c r="B558" s="7" t="s">
         <v>943</v>
       </c>
+      <c r="C558" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D558" t="s">
         <v>1043</v>
       </c>
@@ -14698,6 +14902,9 @@
       <c r="B559" s="7" t="s">
         <v>943</v>
       </c>
+      <c r="C559" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D559" t="s">
         <v>1044</v>
       </c>
@@ -14712,6 +14919,9 @@
       <c r="B560" s="7" t="s">
         <v>943</v>
       </c>
+      <c r="C560" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D560" t="s">
         <v>1045</v>
       </c>
@@ -14723,6 +14933,9 @@
       <c r="B561" s="7" t="s">
         <v>943</v>
       </c>
+      <c r="C561" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D561" t="s">
         <v>1046</v>
       </c>
@@ -14737,6 +14950,9 @@
       <c r="B562" s="7" t="s">
         <v>943</v>
       </c>
+      <c r="C562" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D562" t="s">
         <v>1047</v>
       </c>
@@ -14751,6 +14967,9 @@
       <c r="B563" s="7" t="s">
         <v>943</v>
       </c>
+      <c r="C563" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D563" t="s">
         <v>1048</v>
       </c>
@@ -14765,6 +14984,9 @@
       <c r="B564" s="7" t="s">
         <v>943</v>
       </c>
+      <c r="C564" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D564" t="s">
         <v>1083</v>
       </c>
@@ -14779,6 +15001,9 @@
       <c r="B565" s="7" t="s">
         <v>943</v>
       </c>
+      <c r="C565" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D565" t="s">
         <v>1084</v>
       </c>
@@ -14793,6 +15018,9 @@
       <c r="B566" s="7" t="s">
         <v>943</v>
       </c>
+      <c r="C566" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D566" t="s">
         <v>1085</v>
       </c>
@@ -14804,6 +15032,9 @@
       <c r="B567" s="7" t="s">
         <v>943</v>
       </c>
+      <c r="C567" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D567" t="s">
         <v>1086</v>
       </c>
@@ -14818,6 +15049,9 @@
       <c r="B568" s="7" t="s">
         <v>943</v>
       </c>
+      <c r="C568" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D568" t="s">
         <v>1087</v>
       </c>
@@ -14832,6 +15066,9 @@
       <c r="B569" s="7" t="s">
         <v>943</v>
       </c>
+      <c r="C569" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D569" t="s">
         <v>1088</v>
       </c>
@@ -14846,6 +15083,9 @@
       <c r="B570" s="7" t="s">
         <v>943</v>
       </c>
+      <c r="C570" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D570" t="s">
         <v>1089</v>
       </c>
@@ -14860,6 +15100,9 @@
       <c r="B571" s="7" t="s">
         <v>943</v>
       </c>
+      <c r="C571" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D571" t="s">
         <v>1090</v>
       </c>
@@ -14874,6 +15117,9 @@
       <c r="B572" s="7" t="s">
         <v>943</v>
       </c>
+      <c r="C572" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D572" t="s">
         <v>1091</v>
       </c>
@@ -14888,6 +15134,9 @@
       <c r="B573" s="7" t="s">
         <v>943</v>
       </c>
+      <c r="C573" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D573" t="s">
         <v>1092</v>
       </c>
@@ -14902,6 +15151,9 @@
       <c r="B574" s="7" t="s">
         <v>943</v>
       </c>
+      <c r="C574" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D574" t="s">
         <v>1093</v>
       </c>
@@ -14916,6 +15168,9 @@
       <c r="B575" s="7" t="s">
         <v>943</v>
       </c>
+      <c r="C575" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D575" t="s">
         <v>1094</v>
       </c>
@@ -14930,6 +15185,9 @@
       <c r="B576" s="7" t="s">
         <v>943</v>
       </c>
+      <c r="C576" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D576" t="s">
         <v>1095</v>
       </c>
@@ -14944,6 +15202,9 @@
       <c r="B577" s="7" t="s">
         <v>943</v>
       </c>
+      <c r="C577" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D577" t="s">
         <v>1096</v>
       </c>
@@ -14958,6 +15219,9 @@
       <c r="B578" s="7" t="s">
         <v>943</v>
       </c>
+      <c r="C578" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D578" t="s">
         <v>1097</v>
       </c>
@@ -14972,6 +15236,9 @@
       <c r="B579" t="s">
         <v>1112</v>
       </c>
+      <c r="C579" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D579" t="s">
         <v>1113</v>
       </c>
@@ -14986,6 +15253,9 @@
       <c r="B580" t="s">
         <v>1112</v>
       </c>
+      <c r="C580" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D580" t="s">
         <v>1114</v>
       </c>
@@ -15000,6 +15270,9 @@
       <c r="B581" t="s">
         <v>1112</v>
       </c>
+      <c r="C581" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D581" t="s">
         <v>1115</v>
       </c>
@@ -15014,6 +15287,9 @@
       <c r="B582" t="s">
         <v>1112</v>
       </c>
+      <c r="C582" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D582" t="s">
         <v>1116</v>
       </c>
@@ -15028,6 +15304,9 @@
       <c r="B583" t="s">
         <v>1112</v>
       </c>
+      <c r="C583" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D583" t="s">
         <v>1117</v>
       </c>
@@ -15042,6 +15321,9 @@
       <c r="B584" t="s">
         <v>1112</v>
       </c>
+      <c r="C584" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D584" t="s">
         <v>1118</v>
       </c>
@@ -15056,6 +15338,9 @@
       <c r="B585" t="s">
         <v>1112</v>
       </c>
+      <c r="C585" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D585" t="s">
         <v>1119</v>
       </c>
@@ -15070,6 +15355,9 @@
       <c r="B586" t="s">
         <v>1112</v>
       </c>
+      <c r="C586" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D586" t="s">
         <v>1120</v>
       </c>
@@ -15084,6 +15372,9 @@
       <c r="B587" t="s">
         <v>1112</v>
       </c>
+      <c r="C587" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D587" t="s">
         <v>1121</v>
       </c>
@@ -15098,6 +15389,9 @@
       <c r="B588" t="s">
         <v>1112</v>
       </c>
+      <c r="C588" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D588" t="s">
         <v>1122</v>
       </c>
@@ -15112,6 +15406,9 @@
       <c r="B589" t="s">
         <v>1112</v>
       </c>
+      <c r="C589" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D589" t="s">
         <v>1123</v>
       </c>
@@ -15126,6 +15423,9 @@
       <c r="B590" t="s">
         <v>1112</v>
       </c>
+      <c r="C590" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D590" t="s">
         <v>1124</v>
       </c>
@@ -15140,6 +15440,9 @@
       <c r="B591" t="s">
         <v>1112</v>
       </c>
+      <c r="C591" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D591" t="s">
         <v>1125</v>
       </c>
@@ -15154,6 +15457,9 @@
       <c r="B592" t="s">
         <v>1112</v>
       </c>
+      <c r="C592" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D592" t="s">
         <v>1126</v>
       </c>
@@ -15168,6 +15474,9 @@
       <c r="B593" t="s">
         <v>1112</v>
       </c>
+      <c r="C593" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D593" t="s">
         <v>1127</v>
       </c>
@@ -15182,6 +15491,9 @@
       <c r="B594" t="s">
         <v>1112</v>
       </c>
+      <c r="C594" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D594" t="s">
         <v>1128</v>
       </c>
@@ -15196,6 +15508,9 @@
       <c r="B595" t="s">
         <v>1112</v>
       </c>
+      <c r="C595" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D595" t="s">
         <v>1129</v>
       </c>
@@ -15210,6 +15525,9 @@
       <c r="B596" t="s">
         <v>1112</v>
       </c>
+      <c r="C596" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D596" t="s">
         <v>1130</v>
       </c>
@@ -15224,6 +15542,9 @@
       <c r="B597" t="s">
         <v>1112</v>
       </c>
+      <c r="C597" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D597" t="s">
         <v>1131</v>
       </c>
@@ -15238,6 +15559,9 @@
       <c r="B598" t="s">
         <v>1112</v>
       </c>
+      <c r="C598" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D598" t="s">
         <v>1132</v>
       </c>
@@ -15252,6 +15576,9 @@
       <c r="B599" t="s">
         <v>1112</v>
       </c>
+      <c r="C599" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D599" t="s">
         <v>1133</v>
       </c>
@@ -15266,6 +15593,9 @@
       <c r="B600" t="s">
         <v>1112</v>
       </c>
+      <c r="C600" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D600" t="s">
         <v>1134</v>
       </c>
@@ -15280,6 +15610,9 @@
       <c r="B601" t="s">
         <v>1112</v>
       </c>
+      <c r="C601" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D601" t="s">
         <v>1135</v>
       </c>
@@ -15294,6 +15627,9 @@
       <c r="B602" t="s">
         <v>1112</v>
       </c>
+      <c r="C602" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D602" t="s">
         <v>1136</v>
       </c>
@@ -15308,6 +15644,9 @@
       <c r="B603" t="s">
         <v>1112</v>
       </c>
+      <c r="C603" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D603" t="s">
         <v>1137</v>
       </c>
@@ -15322,6 +15661,9 @@
       <c r="B604" t="s">
         <v>1112</v>
       </c>
+      <c r="C604" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D604" t="s">
         <v>1138</v>
       </c>
@@ -15336,6 +15678,9 @@
       <c r="B605" t="s">
         <v>1112</v>
       </c>
+      <c r="C605" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D605" t="s">
         <v>1139</v>
       </c>
@@ -15350,6 +15695,9 @@
       <c r="B606" t="s">
         <v>1112</v>
       </c>
+      <c r="C606" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D606" t="s">
         <v>1140</v>
       </c>
@@ -15364,6 +15712,9 @@
       <c r="B607" t="s">
         <v>1112</v>
       </c>
+      <c r="C607" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D607" t="s">
         <v>1141</v>
       </c>
@@ -15378,6 +15729,9 @@
       <c r="B608" t="s">
         <v>1112</v>
       </c>
+      <c r="C608" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D608" t="s">
         <v>1142</v>
       </c>
@@ -15392,6 +15746,9 @@
       <c r="B609" t="s">
         <v>1112</v>
       </c>
+      <c r="C609" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D609" t="s">
         <v>1143</v>
       </c>
@@ -15406,6 +15763,9 @@
       <c r="B610" t="s">
         <v>1112</v>
       </c>
+      <c r="C610" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D610" t="s">
         <v>1144</v>
       </c>
@@ -15420,6 +15780,9 @@
       <c r="B611" t="s">
         <v>1112</v>
       </c>
+      <c r="C611" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D611" t="s">
         <v>1145</v>
       </c>
@@ -15434,6 +15797,9 @@
       <c r="B612" t="s">
         <v>1112</v>
       </c>
+      <c r="C612" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D612" t="s">
         <v>1146</v>
       </c>
@@ -15448,6 +15814,9 @@
       <c r="B613" t="s">
         <v>1112</v>
       </c>
+      <c r="C613" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D613" t="s">
         <v>1147</v>
       </c>
@@ -15459,6 +15828,9 @@
       <c r="B614" t="s">
         <v>1112</v>
       </c>
+      <c r="C614" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D614" t="s">
         <v>1148</v>
       </c>
@@ -15473,6 +15845,9 @@
       <c r="B615" t="s">
         <v>1112</v>
       </c>
+      <c r="C615" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D615" t="s">
         <v>1179</v>
       </c>
@@ -15487,6 +15862,9 @@
       <c r="B616" t="s">
         <v>1112</v>
       </c>
+      <c r="C616" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D616" t="s">
         <v>1180</v>
       </c>
@@ -15501,6 +15879,9 @@
       <c r="B617" t="s">
         <v>1112</v>
       </c>
+      <c r="C617" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D617" t="s">
         <v>1181</v>
       </c>
@@ -15515,6 +15896,9 @@
       <c r="B618" t="s">
         <v>1112</v>
       </c>
+      <c r="C618" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D618" t="s">
         <v>1182</v>
       </c>
@@ -15529,6 +15913,9 @@
       <c r="B619" t="s">
         <v>1112</v>
       </c>
+      <c r="C619" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D619" t="s">
         <v>1183</v>
       </c>
@@ -15543,6 +15930,9 @@
       <c r="B620" t="s">
         <v>1112</v>
       </c>
+      <c r="C620" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D620" t="s">
         <v>1184</v>
       </c>
@@ -15557,6 +15947,9 @@
       <c r="B621" t="s">
         <v>1112</v>
       </c>
+      <c r="C621" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D621" t="s">
         <v>1185</v>
       </c>
@@ -15571,6 +15964,9 @@
       <c r="B622" t="s">
         <v>1112</v>
       </c>
+      <c r="C622" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D622" t="s">
         <v>1186</v>
       </c>
@@ -15585,6 +15981,9 @@
       <c r="B623" t="s">
         <v>1112</v>
       </c>
+      <c r="C623" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D623" t="s">
         <v>1187</v>
       </c>
@@ -15599,6 +15998,9 @@
       <c r="B624" t="s">
         <v>1112</v>
       </c>
+      <c r="C624" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D624" t="s">
         <v>1188</v>
       </c>
@@ -15613,6 +16015,9 @@
       <c r="B625" t="s">
         <v>1112</v>
       </c>
+      <c r="C625" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D625" t="s">
         <v>1189</v>
       </c>
@@ -15627,6 +16032,9 @@
       <c r="B626" t="s">
         <v>1112</v>
       </c>
+      <c r="C626" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D626" t="s">
         <v>1190</v>
       </c>
@@ -15641,6 +16049,9 @@
       <c r="B627" t="s">
         <v>1112</v>
       </c>
+      <c r="C627" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D627" t="s">
         <v>1191</v>
       </c>
@@ -15655,6 +16066,9 @@
       <c r="B628" t="s">
         <v>1112</v>
       </c>
+      <c r="C628" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D628" t="s">
         <v>1192</v>
       </c>
@@ -15669,6 +16083,9 @@
       <c r="B629" t="s">
         <v>1112</v>
       </c>
+      <c r="C629" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D629" t="s">
         <v>1193</v>
       </c>
@@ -15683,6 +16100,9 @@
       <c r="B630" t="s">
         <v>1112</v>
       </c>
+      <c r="C630" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D630" t="s">
         <v>1194</v>
       </c>
@@ -15697,6 +16117,9 @@
       <c r="B631" t="s">
         <v>1112</v>
       </c>
+      <c r="C631" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D631" t="s">
         <v>1195</v>
       </c>
@@ -15711,6 +16134,9 @@
       <c r="B632" t="s">
         <v>1112</v>
       </c>
+      <c r="C632" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D632" t="s">
         <v>1196</v>
       </c>
@@ -15725,6 +16151,9 @@
       <c r="B633" t="s">
         <v>1112</v>
       </c>
+      <c r="C633" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D633" t="s">
         <v>1197</v>
       </c>
@@ -15739,6 +16168,9 @@
       <c r="B634" t="s">
         <v>1112</v>
       </c>
+      <c r="C634" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D634" t="s">
         <v>1198</v>
       </c>
@@ -15753,6 +16185,9 @@
       <c r="B635" t="s">
         <v>1112</v>
       </c>
+      <c r="C635" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D635" t="s">
         <v>1199</v>
       </c>
@@ -15767,6 +16202,9 @@
       <c r="B636" t="s">
         <v>1112</v>
       </c>
+      <c r="C636" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D636" t="s">
         <v>1200</v>
       </c>
@@ -15781,6 +16219,9 @@
       <c r="B637" t="s">
         <v>1112</v>
       </c>
+      <c r="C637" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D637" t="s">
         <v>1201</v>
       </c>
@@ -15795,6 +16236,9 @@
       <c r="B638" t="s">
         <v>1112</v>
       </c>
+      <c r="C638" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D638" t="s">
         <v>1202</v>
       </c>
@@ -15809,6 +16253,9 @@
       <c r="B639" t="s">
         <v>1112</v>
       </c>
+      <c r="C639" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D639" t="s">
         <v>1203</v>
       </c>
@@ -15823,6 +16270,9 @@
       <c r="B640" t="s">
         <v>1112</v>
       </c>
+      <c r="C640" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D640" t="s">
         <v>1204</v>
       </c>
@@ -15837,6 +16287,9 @@
       <c r="B641" t="s">
         <v>1112</v>
       </c>
+      <c r="C641" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D641" t="s">
         <v>1205</v>
       </c>
@@ -15851,6 +16304,9 @@
       <c r="B642" t="s">
         <v>1112</v>
       </c>
+      <c r="C642" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D642" t="s">
         <v>1206</v>
       </c>
@@ -15865,6 +16321,9 @@
       <c r="B643" t="s">
         <v>1112</v>
       </c>
+      <c r="C643" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D643" t="s">
         <v>1207</v>
       </c>
@@ -15879,6 +16338,9 @@
       <c r="B644" t="s">
         <v>1112</v>
       </c>
+      <c r="C644" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D644" t="s">
         <v>1208</v>
       </c>
@@ -15893,6 +16355,9 @@
       <c r="B645" t="s">
         <v>1112</v>
       </c>
+      <c r="C645" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D645" t="s">
         <v>1209</v>
       </c>
@@ -15907,6 +16372,9 @@
       <c r="B646" t="s">
         <v>1112</v>
       </c>
+      <c r="C646" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D646" t="s">
         <v>1210</v>
       </c>
@@ -15921,6 +16389,9 @@
       <c r="B647" t="s">
         <v>1112</v>
       </c>
+      <c r="C647" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D647" t="s">
         <v>1211</v>
       </c>
@@ -15935,6 +16406,9 @@
       <c r="B648" t="s">
         <v>1112</v>
       </c>
+      <c r="C648" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D648" t="s">
         <v>1241</v>
       </c>
@@ -15949,6 +16423,9 @@
       <c r="B649" t="s">
         <v>1112</v>
       </c>
+      <c r="C649" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D649" t="s">
         <v>1242</v>
       </c>
@@ -15963,6 +16440,9 @@
       <c r="B650" t="s">
         <v>1112</v>
       </c>
+      <c r="C650" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D650" t="s">
         <v>1243</v>
       </c>
@@ -15977,6 +16457,9 @@
       <c r="B651" t="s">
         <v>1112</v>
       </c>
+      <c r="C651" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D651" t="s">
         <v>1244</v>
       </c>
@@ -15991,6 +16474,9 @@
       <c r="B652" t="s">
         <v>1112</v>
       </c>
+      <c r="C652" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D652" t="s">
         <v>1245</v>
       </c>
@@ -16005,6 +16491,9 @@
       <c r="B653" t="s">
         <v>1112</v>
       </c>
+      <c r="C653" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D653" t="s">
         <v>1246</v>
       </c>
@@ -16019,6 +16508,9 @@
       <c r="B654" t="s">
         <v>1112</v>
       </c>
+      <c r="C654" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D654" t="s">
         <v>1247</v>
       </c>
@@ -16033,6 +16525,9 @@
       <c r="B655" t="s">
         <v>1112</v>
       </c>
+      <c r="C655" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D655" t="s">
         <v>1248</v>
       </c>
@@ -16047,6 +16542,9 @@
       <c r="B656" t="s">
         <v>1112</v>
       </c>
+      <c r="C656" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D656" t="s">
         <v>1249</v>
       </c>
@@ -16061,6 +16559,9 @@
       <c r="B657" t="s">
         <v>1112</v>
       </c>
+      <c r="C657" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D657" t="s">
         <v>1250</v>
       </c>
@@ -16075,6 +16576,9 @@
       <c r="B658" t="s">
         <v>1112</v>
       </c>
+      <c r="C658" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D658" t="s">
         <v>1251</v>
       </c>
@@ -16089,6 +16593,9 @@
       <c r="B659" t="s">
         <v>1112</v>
       </c>
+      <c r="C659" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D659" t="s">
         <v>1252</v>
       </c>
@@ -16103,6 +16610,9 @@
       <c r="B660" t="s">
         <v>1112</v>
       </c>
+      <c r="C660" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D660" t="s">
         <v>1253</v>
       </c>
@@ -16117,6 +16627,9 @@
       <c r="B661" t="s">
         <v>1112</v>
       </c>
+      <c r="C661" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D661" t="s">
         <v>1254</v>
       </c>
@@ -16131,6 +16644,9 @@
       <c r="B662" t="s">
         <v>1269</v>
       </c>
+      <c r="C662" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D662" t="s">
         <v>1270</v>
       </c>
@@ -16145,6 +16661,9 @@
       <c r="B663" t="s">
         <v>1269</v>
       </c>
+      <c r="C663" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D663">
         <v>7805</v>
       </c>
@@ -16159,6 +16678,9 @@
       <c r="B664" t="s">
         <v>1269</v>
       </c>
+      <c r="C664" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D664" t="s">
         <v>1271</v>
       </c>
@@ -16173,6 +16695,9 @@
       <c r="B665" t="s">
         <v>1269</v>
       </c>
+      <c r="C665" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D665" t="s">
         <v>1272</v>
       </c>
@@ -16187,6 +16712,9 @@
       <c r="B666" t="s">
         <v>1269</v>
       </c>
+      <c r="C666" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D666" t="s">
         <v>1273</v>
       </c>
@@ -16201,6 +16729,9 @@
       <c r="B667" t="s">
         <v>1269</v>
       </c>
+      <c r="C667" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D667" t="s">
         <v>1274</v>
       </c>
@@ -16215,6 +16746,9 @@
       <c r="B668" t="s">
         <v>1269</v>
       </c>
+      <c r="C668" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D668" t="s">
         <v>1275</v>
       </c>
@@ -16229,6 +16763,9 @@
       <c r="B669" t="s">
         <v>1269</v>
       </c>
+      <c r="C669" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D669" t="s">
         <v>1276</v>
       </c>
@@ -16243,6 +16780,9 @@
       <c r="B670" t="s">
         <v>1269</v>
       </c>
+      <c r="C670" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D670" t="s">
         <v>1277</v>
       </c>
@@ -16257,6 +16797,9 @@
       <c r="B671" t="s">
         <v>1269</v>
       </c>
+      <c r="C671" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D671" t="s">
         <v>1278</v>
       </c>
@@ -16271,6 +16814,9 @@
       <c r="B672" t="s">
         <v>1269</v>
       </c>
+      <c r="C672" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D672" t="s">
         <v>1279</v>
       </c>
@@ -16285,6 +16831,9 @@
       <c r="B673" t="s">
         <v>1269</v>
       </c>
+      <c r="C673" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D673" t="s">
         <v>1280</v>
       </c>
@@ -16299,6 +16848,9 @@
       <c r="B674" t="s">
         <v>1269</v>
       </c>
+      <c r="C674" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D674" t="s">
         <v>1281</v>
       </c>
@@ -16313,6 +16865,9 @@
       <c r="B675" t="s">
         <v>1269</v>
       </c>
+      <c r="C675" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D675" t="s">
         <v>1282</v>
       </c>
@@ -16327,6 +16882,9 @@
       <c r="B676" t="s">
         <v>1269</v>
       </c>
+      <c r="C676" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D676" t="s">
         <v>1283</v>
       </c>
@@ -16341,6 +16899,9 @@
       <c r="B677" t="s">
         <v>1269</v>
       </c>
+      <c r="C677" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D677" t="s">
         <v>1284</v>
       </c>
@@ -16355,6 +16916,9 @@
       <c r="B678" t="s">
         <v>1269</v>
       </c>
+      <c r="C678" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D678" t="s">
         <v>1285</v>
       </c>
@@ -16369,6 +16933,9 @@
       <c r="B679" t="s">
         <v>1269</v>
       </c>
+      <c r="C679" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D679" t="s">
         <v>1286</v>
       </c>
@@ -16383,6 +16950,9 @@
       <c r="B680" t="s">
         <v>1269</v>
       </c>
+      <c r="C680" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D680" t="s">
         <v>1287</v>
       </c>
@@ -16397,6 +16967,9 @@
       <c r="B681" t="s">
         <v>1269</v>
       </c>
+      <c r="C681" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D681" t="s">
         <v>1288</v>
       </c>
@@ -16411,6 +16984,9 @@
       <c r="B682" t="s">
         <v>1309</v>
       </c>
+      <c r="C682" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D682" t="s">
         <v>1310</v>
       </c>
@@ -16425,6 +17001,9 @@
       <c r="B683" t="s">
         <v>1309</v>
       </c>
+      <c r="C683" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D683" t="s">
         <v>1311</v>
       </c>
@@ -16439,6 +17018,9 @@
       <c r="B684" t="s">
         <v>1309</v>
       </c>
+      <c r="C684" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D684" t="s">
         <v>1312</v>
       </c>
@@ -16453,6 +17035,9 @@
       <c r="B685" t="s">
         <v>1309</v>
       </c>
+      <c r="C685" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D685" t="s">
         <v>1313</v>
       </c>
@@ -16467,6 +17052,9 @@
       <c r="B686" t="s">
         <v>1309</v>
       </c>
+      <c r="C686" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D686" t="s">
         <v>1314</v>
       </c>
@@ -16481,6 +17069,9 @@
       <c r="B687" t="s">
         <v>1369</v>
       </c>
+      <c r="C687" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D687" t="s">
         <v>1320</v>
       </c>
@@ -16495,6 +17086,9 @@
       <c r="B688" t="s">
         <v>1369</v>
       </c>
+      <c r="C688" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D688" t="s">
         <v>1321</v>
       </c>
@@ -16509,6 +17103,9 @@
       <c r="B689" t="s">
         <v>1369</v>
       </c>
+      <c r="C689" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D689" t="s">
         <v>1322</v>
       </c>
@@ -16523,6 +17120,9 @@
       <c r="B690" t="s">
         <v>1369</v>
       </c>
+      <c r="C690" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D690" t="s">
         <v>1323</v>
       </c>
@@ -16537,6 +17137,9 @@
       <c r="B691" t="s">
         <v>1369</v>
       </c>
+      <c r="C691" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D691" t="s">
         <v>1324</v>
       </c>
@@ -16551,6 +17154,9 @@
       <c r="B692" t="s">
         <v>1369</v>
       </c>
+      <c r="C692" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D692" t="s">
         <v>1325</v>
       </c>
@@ -16565,6 +17171,9 @@
       <c r="B693" t="s">
         <v>1369</v>
       </c>
+      <c r="C693" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D693" t="s">
         <v>1326</v>
       </c>
@@ -16579,6 +17188,9 @@
       <c r="B694" t="s">
         <v>1369</v>
       </c>
+      <c r="C694" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D694" t="s">
         <v>1327</v>
       </c>
@@ -16593,6 +17205,9 @@
       <c r="B695" t="s">
         <v>1369</v>
       </c>
+      <c r="C695" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D695" t="s">
         <v>1328</v>
       </c>
@@ -16607,6 +17222,9 @@
       <c r="B696" t="s">
         <v>1369</v>
       </c>
+      <c r="C696" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D696" t="s">
         <v>1329</v>
       </c>
@@ -16621,6 +17239,9 @@
       <c r="B697" t="s">
         <v>1369</v>
       </c>
+      <c r="C697" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D697" t="s">
         <v>1330</v>
       </c>
@@ -16635,6 +17256,9 @@
       <c r="B698" t="s">
         <v>1369</v>
       </c>
+      <c r="C698" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D698" t="s">
         <v>1331</v>
       </c>
@@ -16649,6 +17273,9 @@
       <c r="B699" t="s">
         <v>1369</v>
       </c>
+      <c r="C699" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D699" t="s">
         <v>1332</v>
       </c>
@@ -16663,6 +17290,9 @@
       <c r="B700" t="s">
         <v>1369</v>
       </c>
+      <c r="C700" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D700" t="s">
         <v>1333</v>
       </c>
@@ -16677,6 +17307,9 @@
       <c r="B701" t="s">
         <v>1369</v>
       </c>
+      <c r="C701" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D701" t="s">
         <v>1334</v>
       </c>
@@ -16691,6 +17324,9 @@
       <c r="B702" t="s">
         <v>1369</v>
       </c>
+      <c r="C702" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D702" t="s">
         <v>1335</v>
       </c>
@@ -16705,6 +17341,9 @@
       <c r="B703" t="s">
         <v>1369</v>
       </c>
+      <c r="C703" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D703" t="s">
         <v>1336</v>
       </c>
@@ -16719,6 +17358,9 @@
       <c r="B704" t="s">
         <v>1369</v>
       </c>
+      <c r="C704" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D704" t="s">
         <v>1337</v>
       </c>
@@ -16733,6 +17375,9 @@
       <c r="B705" t="s">
         <v>1369</v>
       </c>
+      <c r="C705" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D705" t="s">
         <v>1338</v>
       </c>
@@ -16747,6 +17392,9 @@
       <c r="B706" t="s">
         <v>1369</v>
       </c>
+      <c r="C706" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D706" t="s">
         <v>1339</v>
       </c>
@@ -16761,6 +17409,9 @@
       <c r="B707" t="s">
         <v>1369</v>
       </c>
+      <c r="C707" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D707" t="s">
         <v>1340</v>
       </c>
@@ -16775,6 +17426,9 @@
       <c r="B708" t="s">
         <v>1369</v>
       </c>
+      <c r="C708" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D708" t="s">
         <v>1341</v>
       </c>
@@ -16789,6 +17443,9 @@
       <c r="B709" t="s">
         <v>1369</v>
       </c>
+      <c r="C709" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D709" t="s">
         <v>1342</v>
       </c>
@@ -16803,6 +17460,9 @@
       <c r="B710" t="s">
         <v>1369</v>
       </c>
+      <c r="C710" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D710" t="s">
         <v>1343</v>
       </c>
@@ -16817,6 +17477,9 @@
       <c r="B711" t="s">
         <v>1369</v>
       </c>
+      <c r="C711" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D711" t="s">
         <v>1344</v>
       </c>
@@ -16831,6 +17494,9 @@
       <c r="B712" t="s">
         <v>1370</v>
       </c>
+      <c r="C712" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D712" t="s">
         <v>1371</v>
       </c>
@@ -16845,6 +17511,9 @@
       <c r="B713" t="s">
         <v>1370</v>
       </c>
+      <c r="C713" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D713" t="s">
         <v>1372</v>
       </c>
@@ -16859,6 +17528,9 @@
       <c r="B714" t="s">
         <v>1370</v>
       </c>
+      <c r="C714" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D714" t="s">
         <v>1373</v>
       </c>
@@ -16873,6 +17545,9 @@
       <c r="B715" t="s">
         <v>1370</v>
       </c>
+      <c r="C715" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D715" t="s">
         <v>1374</v>
       </c>
@@ -16887,6 +17562,9 @@
       <c r="B716" t="s">
         <v>1370</v>
       </c>
+      <c r="C716" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D716" t="s">
         <v>1375</v>
       </c>
@@ -16901,6 +17579,9 @@
       <c r="B717" t="s">
         <v>1370</v>
       </c>
+      <c r="C717" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D717" t="s">
         <v>1376</v>
       </c>
@@ -16915,6 +17596,9 @@
       <c r="B718" t="s">
         <v>1370</v>
       </c>
+      <c r="C718" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D718" t="s">
         <v>1377</v>
       </c>
@@ -16929,6 +17613,9 @@
       <c r="B719" t="s">
         <v>1370</v>
       </c>
+      <c r="C719" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D719" t="s">
         <v>1378</v>
       </c>
@@ -16943,6 +17630,9 @@
       <c r="B720" t="s">
         <v>1370</v>
       </c>
+      <c r="C720" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D720" t="s">
         <v>1379</v>
       </c>
@@ -16957,6 +17647,9 @@
       <c r="B721" t="s">
         <v>1370</v>
       </c>
+      <c r="C721" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D721" t="s">
         <v>1380</v>
       </c>
@@ -16971,6 +17664,9 @@
       <c r="B722" t="s">
         <v>1370</v>
       </c>
+      <c r="C722" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D722" t="s">
         <v>1381</v>
       </c>
@@ -16985,6 +17681,9 @@
       <c r="B723" t="s">
         <v>1370</v>
       </c>
+      <c r="C723" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D723" t="s">
         <v>1382</v>
       </c>
@@ -16999,6 +17698,9 @@
       <c r="B724" t="s">
         <v>1370</v>
       </c>
+      <c r="C724" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D724" t="s">
         <v>1383</v>
       </c>
@@ -17013,6 +17715,9 @@
       <c r="B725" t="s">
         <v>1370</v>
       </c>
+      <c r="C725" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D725" t="s">
         <v>1384</v>
       </c>
@@ -17027,6 +17732,9 @@
       <c r="B726" t="s">
         <v>1370</v>
       </c>
+      <c r="C726" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D726" t="s">
         <v>1385</v>
       </c>
@@ -17041,6 +17749,9 @@
       <c r="B727" t="s">
         <v>1399</v>
       </c>
+      <c r="C727" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D727" t="s">
         <v>1400</v>
       </c>
@@ -17055,6 +17766,9 @@
       <c r="B728" t="s">
         <v>1399</v>
       </c>
+      <c r="C728" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D728" t="s">
         <v>1401</v>
       </c>
@@ -17069,6 +17783,9 @@
       <c r="B729" t="s">
         <v>1399</v>
       </c>
+      <c r="C729" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D729" t="s">
         <v>1402</v>
       </c>
@@ -17083,6 +17800,9 @@
       <c r="B730" t="s">
         <v>1399</v>
       </c>
+      <c r="C730" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D730" t="s">
         <v>1403</v>
       </c>
@@ -17097,6 +17817,9 @@
       <c r="B731" t="s">
         <v>1399</v>
       </c>
+      <c r="C731" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D731" t="s">
         <v>1404</v>
       </c>
@@ -17111,6 +17834,9 @@
       <c r="B732" t="s">
         <v>1399</v>
       </c>
+      <c r="C732" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D732" t="s">
         <v>1405</v>
       </c>
@@ -17125,6 +17851,9 @@
       <c r="B733" t="s">
         <v>1399</v>
       </c>
+      <c r="C733" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D733" t="s">
         <v>1406</v>
       </c>
@@ -17139,6 +17868,9 @@
       <c r="B734" t="s">
         <v>1399</v>
       </c>
+      <c r="C734" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D734" t="s">
         <v>1407</v>
       </c>
@@ -17153,6 +17885,9 @@
       <c r="B735" t="s">
         <v>1399</v>
       </c>
+      <c r="C735" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D735" t="s">
         <v>1408</v>
       </c>
@@ -17167,6 +17902,9 @@
       <c r="B736" t="s">
         <v>1399</v>
       </c>
+      <c r="C736" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D736" t="s">
         <v>1409</v>
       </c>
@@ -17181,6 +17919,9 @@
       <c r="B737" t="s">
         <v>1399</v>
       </c>
+      <c r="C737" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D737" t="s">
         <v>1410</v>
       </c>
@@ -17195,6 +17936,9 @@
       <c r="B738" t="s">
         <v>1399</v>
       </c>
+      <c r="C738" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D738" t="s">
         <v>1411</v>
       </c>
@@ -17209,6 +17953,9 @@
       <c r="B739" t="s">
         <v>1399</v>
       </c>
+      <c r="C739" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D739" t="s">
         <v>1412</v>
       </c>
@@ -17223,6 +17970,9 @@
       <c r="B740" t="s">
         <v>1399</v>
       </c>
+      <c r="C740" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D740" t="s">
         <v>1413</v>
       </c>
@@ -17237,6 +17987,9 @@
       <c r="B741" t="s">
         <v>1399</v>
       </c>
+      <c r="C741" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D741" t="s">
         <v>1414</v>
       </c>
@@ -17251,6 +18004,9 @@
       <c r="B742" t="s">
         <v>1399</v>
       </c>
+      <c r="C742" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D742" t="s">
         <v>1415</v>
       </c>
@@ -17265,6 +18021,9 @@
       <c r="B743" t="s">
         <v>1399</v>
       </c>
+      <c r="C743" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D743" t="s">
         <v>1416</v>
       </c>
@@ -17279,6 +18038,9 @@
       <c r="B744" t="s">
         <v>1399</v>
       </c>
+      <c r="C744" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D744" t="s">
         <v>1417</v>
       </c>
@@ -17293,6 +18055,9 @@
       <c r="B745" t="s">
         <v>1399</v>
       </c>
+      <c r="C745" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D745" t="s">
         <v>1418</v>
       </c>
@@ -17307,6 +18072,9 @@
       <c r="B746" t="s">
         <v>1438</v>
       </c>
+      <c r="C746" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D746" t="s">
         <v>1439</v>
       </c>
@@ -17321,6 +18089,9 @@
       <c r="B747" t="s">
         <v>1438</v>
       </c>
+      <c r="C747" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D747" t="s">
         <v>1440</v>
       </c>
@@ -17335,6 +18106,9 @@
       <c r="B748" t="s">
         <v>1438</v>
       </c>
+      <c r="C748" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D748" t="s">
         <v>1441</v>
       </c>
@@ -17349,6 +18123,9 @@
       <c r="B749" t="s">
         <v>1438</v>
       </c>
+      <c r="C749" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D749" t="s">
         <v>1442</v>
       </c>
@@ -17363,6 +18140,9 @@
       <c r="B750" t="s">
         <v>1438</v>
       </c>
+      <c r="C750" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D750" t="s">
         <v>1443</v>
       </c>
@@ -17377,6 +18157,9 @@
       <c r="B751" t="s">
         <v>1438</v>
       </c>
+      <c r="C751" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D751" t="s">
         <v>1444</v>
       </c>
@@ -17391,6 +18174,9 @@
       <c r="B752" t="s">
         <v>1438</v>
       </c>
+      <c r="C752" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D752" t="s">
         <v>1445</v>
       </c>
@@ -17405,6 +18191,9 @@
       <c r="B753" t="s">
         <v>1438</v>
       </c>
+      <c r="C753" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D753" t="s">
         <v>1446</v>
       </c>
@@ -17419,6 +18208,9 @@
       <c r="B754" t="s">
         <v>1438</v>
       </c>
+      <c r="C754" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D754" t="s">
         <v>1447</v>
       </c>
@@ -17433,6 +18225,9 @@
       <c r="B755" t="s">
         <v>1438</v>
       </c>
+      <c r="C755" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D755" t="s">
         <v>1448</v>
       </c>
@@ -17447,6 +18242,9 @@
       <c r="B756" t="s">
         <v>1438</v>
       </c>
+      <c r="C756" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D756" t="s">
         <v>1449</v>
       </c>
@@ -17461,6 +18259,9 @@
       <c r="B757" t="s">
         <v>1438</v>
       </c>
+      <c r="C757" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D757" t="s">
         <v>1450</v>
       </c>
@@ -17475,6 +18276,9 @@
       <c r="B758" t="s">
         <v>1461</v>
       </c>
+      <c r="C758" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D758" t="s">
         <v>1462</v>
       </c>
@@ -17489,6 +18293,9 @@
       <c r="B759" t="s">
         <v>1461</v>
       </c>
+      <c r="C759" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D759" t="s">
         <v>1463</v>
       </c>
@@ -17503,6 +18310,9 @@
       <c r="B760" t="s">
         <v>1461</v>
       </c>
+      <c r="C760" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D760" t="s">
         <v>1464</v>
       </c>
@@ -17517,6 +18327,9 @@
       <c r="B761" t="s">
         <v>1461</v>
       </c>
+      <c r="C761" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D761" t="s">
         <v>1465</v>
       </c>
@@ -17531,6 +18344,9 @@
       <c r="B762" t="s">
         <v>1461</v>
       </c>
+      <c r="C762" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D762" t="s">
         <v>1466</v>
       </c>
@@ -17545,6 +18361,9 @@
       <c r="B763" t="s">
         <v>1461</v>
       </c>
+      <c r="C763" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D763" t="s">
         <v>1467</v>
       </c>
@@ -17559,6 +18378,9 @@
       <c r="B764" t="s">
         <v>1461</v>
       </c>
+      <c r="C764" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D764" t="s">
         <v>1468</v>
       </c>
@@ -17573,6 +18395,9 @@
       <c r="B765" t="s">
         <v>1461</v>
       </c>
+      <c r="C765" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D765" t="s">
         <v>1469</v>
       </c>
@@ -17587,6 +18412,9 @@
       <c r="B766" t="s">
         <v>1461</v>
       </c>
+      <c r="C766" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D766" t="s">
         <v>1470</v>
       </c>
@@ -17601,6 +18429,9 @@
       <c r="B767" t="s">
         <v>1461</v>
       </c>
+      <c r="C767" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D767" t="s">
         <v>1471</v>
       </c>
@@ -17615,6 +18446,9 @@
       <c r="B768" t="s">
         <v>1461</v>
       </c>
+      <c r="C768" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D768" t="s">
         <v>1472</v>
       </c>
@@ -17629,6 +18463,9 @@
       <c r="B769" t="s">
         <v>1461</v>
       </c>
+      <c r="C769" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D769" t="s">
         <v>1473</v>
       </c>
@@ -17643,6 +18480,9 @@
       <c r="B770" t="s">
         <v>1461</v>
       </c>
+      <c r="C770" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D770" t="s">
         <v>1474</v>
       </c>
@@ -17657,6 +18497,9 @@
       <c r="B771" t="s">
         <v>1461</v>
       </c>
+      <c r="C771" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D771" t="s">
         <v>1475</v>
       </c>
@@ -17671,6 +18514,9 @@
       <c r="B772" t="s">
         <v>1461</v>
       </c>
+      <c r="C772" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D772" t="s">
         <v>1476</v>
       </c>
@@ -17685,6 +18531,9 @@
       <c r="B773" t="s">
         <v>1492</v>
       </c>
+      <c r="C773" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D773" t="s">
         <v>1493</v>
       </c>
@@ -17699,6 +18548,9 @@
       <c r="B774" t="s">
         <v>1492</v>
       </c>
+      <c r="C774" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D774" t="s">
         <v>1494</v>
       </c>
@@ -17713,6 +18565,9 @@
       <c r="B775" t="s">
         <v>1492</v>
       </c>
+      <c r="C775" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D775" t="s">
         <v>1495</v>
       </c>
@@ -17727,6 +18582,9 @@
       <c r="B776" t="s">
         <v>1492</v>
       </c>
+      <c r="C776" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D776" t="s">
         <v>1496</v>
       </c>
@@ -17741,6 +18599,9 @@
       <c r="B777" t="s">
         <v>1492</v>
       </c>
+      <c r="C777" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D777" t="s">
         <v>1497</v>
       </c>
@@ -17755,6 +18616,9 @@
       <c r="B778" t="s">
         <v>1492</v>
       </c>
+      <c r="C778" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D778" t="s">
         <v>1498</v>
       </c>
@@ -17769,6 +18633,9 @@
       <c r="B779" t="s">
         <v>1492</v>
       </c>
+      <c r="C779" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D779" t="s">
         <v>1499</v>
       </c>
@@ -17783,6 +18650,9 @@
       <c r="B780" t="s">
         <v>1492</v>
       </c>
+      <c r="C780" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D780" t="s">
         <v>1500</v>
       </c>
@@ -17797,6 +18667,9 @@
       <c r="B781" t="s">
         <v>1492</v>
       </c>
+      <c r="C781" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D781" t="s">
         <v>1501</v>
       </c>
@@ -17811,6 +18684,9 @@
       <c r="B782" t="s">
         <v>1492</v>
       </c>
+      <c r="C782" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D782" t="s">
         <v>1502</v>
       </c>
@@ -17825,6 +18701,9 @@
       <c r="B783" t="s">
         <v>1492</v>
       </c>
+      <c r="C783" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D783" t="s">
         <v>1503</v>
       </c>
@@ -17839,6 +18718,9 @@
       <c r="B784" t="s">
         <v>1492</v>
       </c>
+      <c r="C784" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D784" t="s">
         <v>1504</v>
       </c>
@@ -17853,6 +18735,9 @@
       <c r="B785" t="s">
         <v>1492</v>
       </c>
+      <c r="C785" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D785" t="s">
         <v>1505</v>
       </c>
@@ -17867,6 +18752,9 @@
       <c r="B786" t="s">
         <v>1492</v>
       </c>
+      <c r="C786" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D786" t="s">
         <v>1506</v>
       </c>
@@ -17881,6 +18769,9 @@
       <c r="B787" t="s">
         <v>1492</v>
       </c>
+      <c r="C787" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D787" t="s">
         <v>1507</v>
       </c>
@@ -17895,6 +18786,9 @@
       <c r="B788" t="s">
         <v>1492</v>
       </c>
+      <c r="C788" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D788" t="s">
         <v>1508</v>
       </c>
@@ -17909,6 +18803,9 @@
       <c r="B789" t="s">
         <v>1525</v>
       </c>
+      <c r="C789" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D789" t="s">
         <v>1526</v>
       </c>
@@ -17923,6 +18820,9 @@
       <c r="B790" t="s">
         <v>1525</v>
       </c>
+      <c r="C790" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D790" t="s">
         <v>1528</v>
       </c>
@@ -17937,6 +18837,9 @@
       <c r="B791" t="s">
         <v>1529</v>
       </c>
+      <c r="C791" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D791" t="s">
         <v>1530</v>
       </c>
@@ -17951,6 +18854,9 @@
       <c r="B792" t="s">
         <v>1529</v>
       </c>
+      <c r="C792" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D792" t="s">
         <v>1532</v>
       </c>
@@ -17965,6 +18871,9 @@
       <c r="B793" t="s">
         <v>1529</v>
       </c>
+      <c r="C793" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D793" t="s">
         <v>1534</v>
       </c>
@@ -17979,6 +18888,9 @@
       <c r="B794" t="s">
         <v>1529</v>
       </c>
+      <c r="C794" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D794" t="s">
         <v>1536</v>
       </c>
@@ -17993,6 +18905,9 @@
       <c r="B795" t="s">
         <v>1529</v>
       </c>
+      <c r="C795" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D795" t="s">
         <v>1538</v>
       </c>
@@ -18007,6 +18922,9 @@
       <c r="B796" t="s">
         <v>1540</v>
       </c>
+      <c r="C796" s="7" t="s">
+        <v>1545</v>
+      </c>
       <c r="D796" t="s">
         <v>1541</v>
       </c>
@@ -18020,6 +18938,9 @@
     <row r="797" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B797" t="s">
         <v>1540</v>
+      </c>
+      <c r="C797" s="7" t="s">
+        <v>1545</v>
       </c>
       <c r="D797" t="s">
         <v>1543</v>

</xml_diff>